<commit_message>
Other templates from Stephanie for testing
</commit_message>
<xml_diff>
--- a/e8-template-untouched.xlsx
+++ b/e8-template-untouched.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StephanieInfante\Desktop\thursday\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32BEA30-289F-4E18-B483-7590007C85C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A51752-66A8-4A26-90DA-1D4BBA307F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="3" activeTab="14" xr2:uid="{149B6D2C-B18F-46C6-A9A2-8B48A3F23525}"/>
+    <workbookView xWindow="3405" yWindow="2220" windowWidth="34635" windowHeight="15435" firstSheet="2" activeTab="2" xr2:uid="{149B6D2C-B18F-46C6-A9A2-8B48A3F23525}"/>
   </bookViews>
   <sheets>
     <sheet name="1-DoesMyAgencyNeedtoComplete" sheetId="13" r:id="rId1"/>
@@ -31,16 +31,9 @@
     <sheet name="data" sheetId="24" state="hidden" r:id="rId16"/>
     <sheet name="2021Readme" sheetId="3" state="hidden" r:id="rId17"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId18"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'1-DoesMyAgencyNeedtoComplete'!$A$1:$I$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'2-AboutYourAgency'!$A$2:$C$14</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">PolicyR2[#All]</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">PolicyR4[#All]</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">PolicyR5[#All]</definedName>
-    <definedName name="qgea_target_status">[1]Reference!$A$14:$A$21</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1906,7 +1899,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1948,8 +1941,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -2204,6 +2203,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2222,7 +2239,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyAlignment="1">
@@ -2311,9 +2328,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2500,12 +2514,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2627,6 +2635,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2657,9 +2695,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2669,33 +2704,6 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2705,12 +2713,45 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2729,38 +2770,38 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="8" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="8" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -2777,7 +2818,7 @@
     <cellStyle name="Normal 4" xfId="9" xr:uid="{EB67A1A0-AB19-8041-A0FA-222E62834CE1}"/>
     <cellStyle name="Note 2" xfId="6" xr:uid="{9C2FA45C-3CCF-4DE1-B1D2-C7003E085B02}"/>
   </cellStyles>
-  <dxfs count="158">
+  <dxfs count="146">
     <dxf>
       <font>
         <strike val="0"/>
@@ -6352,297 +6393,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -7086,53 +6836,18 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Information Standards"/>
-      <sheetName val="QGEA Policies"/>
-      <sheetName val="Reference"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DF8C5074-499C-744E-971A-9067CECB866C}" name="AboutYou" displayName="AboutYou" ref="A2:C14" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="157">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DF8C5074-499C-744E-971A-9067CECB866C}" name="AboutYou" displayName="AboutYou" ref="A2:C14" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="145">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4E22ACC3-A136-674F-AB2D-C0E12934FA92}" name="Column1" headerRowDxfId="156" headerRowCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{A84757E2-8B75-DD4F-BA7E-51A1C5304BC6}" name="Column2" headerRowDxfId="155"/>
-    <tableColumn id="3" xr3:uid="{A3359D3C-AD18-CA44-B273-35C1342584DD}" name="Column3" headerRowDxfId="154"/>
+    <tableColumn id="1" xr3:uid="{4E22ACC3-A136-674F-AB2D-C0E12934FA92}" name="Column1" headerRowDxfId="144" headerRowCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{A84757E2-8B75-DD4F-BA7E-51A1C5304BC6}" name="Column2" headerRowDxfId="143"/>
+    <tableColumn id="3" xr3:uid="{A3359D3C-AD18-CA44-B273-35C1342584DD}" name="Column3" headerRowDxfId="142"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6164995D-5379-4B4B-AB4D-A1F7140BC99E}" name="PolicyR3e85" displayName="PolicyR3e85" ref="A26:H27" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" headerRowCellStyle="Normal 2" dataCellStyle="20% - Accent2">
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{CE9FC516-AA87-AA47-BBE7-F770B6728414}" name="PR3-E8.5" dataDxfId="58" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{3669DB3C-1E3A-F141-8792-A74B75841706}" name="Disable untrusted Microsoft Office macros_x000a_Macros are increasingly being used to enable the download of malware.  Adversaries can then access sensitive information, so macros should be secured or disabled" dataDxfId="57" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{C2DABD41-D65D-6641-A127-793B0DC3048B}" name="Additional" dataDxfId="56" dataCellStyle="Normal 2"/>
-    <tableColumn id="4" xr3:uid="{DAAAA271-77B9-AB4B-AAAC-5A162EBFE138}" name="Percentage of fleet with MS Office macros disabled. _x000a_(Compute devices where MSOffice installed are considered 'disabled')" dataDxfId="55" dataCellStyle="20% - Accent2"/>
-    <tableColumn id="5" xr3:uid="{7CEE5809-E85B-2448-AEF5-AC9430FD3194}" name="Risk mitigation for macro enabled workstations (evidence may be required)" dataDxfId="54" dataCellStyle="Note 2"/>
-    <tableColumn id="6" xr3:uid="{E4051793-5F59-9248-B72A-8CE003B38081}" name="Additional Comments (optional)" dataDxfId="53" dataCellStyle="Note 2"/>
-    <tableColumn id="7" xr3:uid="{727CBA5F-574C-9845-BC3A-8F1BDF08B84A}" name="Total percentage of protected fleet   (Cybersecurity Unit to review and accept)" dataDxfId="52" dataCellStyle="20% - Accent2"/>
-    <tableColumn id="8" xr3:uid="{CE3B73D5-AE0F-4B4B-813D-F000612DF1E9}" name="Comments if any" dataDxfId="51" dataCellStyle="20% - Accent2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{70ECD7F6-D6AC-3240-8218-56049DE4BA7F}" name="PolicyR3e86" displayName="PolicyR3e86" ref="A29:I30" totalsRowShown="0" headerRowDxfId="50" headerRowCellStyle="Normal 2">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{ABD558FE-5405-D043-B5BB-041AE84D59F0}" name="PR3-E8.6" dataDxfId="49" dataCellStyle="Normal 2"/>
@@ -7149,7 +6864,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{1CBC12C9-0E29-CF4D-A38C-72F34E4C71C3}" name="PolicyR3e87" displayName="PolicyR3e87" ref="A32:H36" totalsRowShown="0" headerRowDxfId="40" headerRowCellStyle="Normal 2">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B08649A6-9535-7B4B-9424-F2639303533F}" name="PR3-E8.7" dataDxfId="39" dataCellStyle="Normal 2"/>
@@ -7165,7 +6880,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{DB2CE024-B531-E342-9F15-E0DD01332C25}" name="PolicyR3e88" displayName="PolicyR3e88" ref="A38:I40" totalsRowShown="0" headerRowDxfId="31" headerRowCellStyle="Normal 2">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{DA115D66-DA77-C34E-8E5E-B8F3C0C102A3}" name="PR3-E8.8" dataDxfId="30" dataCellStyle="Normal 2"/>
@@ -7182,7 +6897,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{031FE43E-217C-2649-AC5F-7A44C958A7D1}" name="PolicyR4" displayName="PolicyR4" ref="A1:G4" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17" headerRowCellStyle="Normal 2">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6E1EDF40-70B6-544B-A986-5E60024AA3D5}" name="#" dataDxfId="16" dataCellStyle="Normal 2"/>
@@ -7197,7 +6912,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{958D11D4-E02A-7043-8E35-69B8DE22E019}" name="PolicyR5" displayName="PolicyR5" ref="A1:E2" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5" headerRowCellStyle="Normal 2">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8E19B852-1D8F-5B41-B909-40400D58B70B}" name="#" dataDxfId="4" dataCellStyle="Normal 2"/>
@@ -7211,24 +6926,6 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92CF42CC-BDE6-4F5E-8166-FF3F2344F966}" name="Table1" displayName="Table1" ref="A1:J4" totalsRowShown="0" headerRowDxfId="153" dataDxfId="152" headerRowCellStyle="Normal 2">
-  <tableColumns count="10">
-    <tableColumn id="3" xr3:uid="{8A35A1E8-53AD-40CA-8B12-B4E66046888B}" name="How are you providing assurance for your ISMS?_x000a_(Choose one option below)" dataDxfId="151" dataCellStyle="Comma"/>
-    <tableColumn id="1" xr3:uid="{4178B884-E6A5-4C91-BB96-D650916A7A5C}" name="I need to provide" dataDxfId="150"/>
-    <tableColumn id="8" xr3:uid="{FD04D785-55CE-B947-9CB4-2DE8F42FFF5A}" name="PR1  -Evidence of ISMS" dataDxfId="149" dataCellStyle="Comma"/>
-    <tableColumn id="2" xr3:uid="{40BF6F44-F42A-6244-A826-0C71E8F6D5AA}" name="PR2 - Risk Management" dataDxfId="148" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{85534739-7B56-974B-B74F-49A1E76CDE3A}" name="PR3  QGISCF,QGAF,DES" dataDxfId="147" dataCellStyle="Comma"/>
-    <tableColumn id="10" xr3:uid="{1AA3EEDB-3446-2E47-9E0E-C0585920D63A}" name="PR3 -E8" dataDxfId="146" dataCellStyle="Comma"/>
-    <tableColumn id="11" xr3:uid="{4722A31D-AA83-4549-BDDE-12FCA0C36BED}" name="PR4 -System Assurance" dataDxfId="145" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{1100E9E9-D361-D843-A5BE-22828356B3BD}" name="PR5 - Accountable Officer Attestation" dataDxfId="144" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{9200340B-BE2B-4576-A979-BF66CDDFDCA8}" name="Guidance" dataDxfId="143" dataCellStyle="Normal 2"/>
-    <tableColumn id="7" xr3:uid="{7B8E8A8E-9B34-41C8-A2E0-502BA653925F}" name="__PowerAppsId__" dataDxfId="142" dataCellStyle="Normal 2"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BF8D1954-0527-4D54-A6C1-7BED95F1568B}" name="PolicyR1" displayName="PolicyR1" ref="A1:I16" totalsRowShown="0" headerRowDxfId="141" dataDxfId="140" tableBorderDxfId="139">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C1D6B8ED-F221-4E0B-871A-CAE3855BB0B1}" name="#" dataDxfId="138" dataCellStyle="Normal 2"/>
@@ -7245,7 +6942,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{2950E7F6-02D7-764D-A273-EA2A6DD44391}" name="PolicyR2" displayName="PolicyR2" ref="A1:G3" totalsRowShown="0" headerRowDxfId="129" headerRowCellStyle="Normal 2">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FA59F3E7-505F-2F40-BAFE-861E26F2EE8D}" name="#" dataDxfId="128" dataCellStyle="Normal 2"/>
@@ -7260,7 +6957,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{267DBBEC-EBD9-8047-934C-46C6794C5CA2}" name="PolicyR3" displayName="PolicyR3" ref="A1:H6" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{EE3C1643-5589-964D-864E-7B73D51F5975}" name="PR3" dataDxfId="119"/>
@@ -7276,7 +6973,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{B5BAC64C-6737-4744-A0F0-64FF9F317168}" name="PolicyR3e81" displayName="PolicyR3e81" ref="A10:F12" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110" tableBorderDxfId="109" headerRowCellStyle="Normal 2">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{0AD3CA88-D8A3-F74D-A507-4590E23BBBF8}" name="PR3- E8.1" dataDxfId="108" dataCellStyle="Normal 2"/>
@@ -7290,7 +6987,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4A653377-3B06-4E4A-B9FE-6F7AFAEF870E}" name="PolicyR3e82" displayName="PolicyR3e82" ref="A14:K16" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101" tableBorderDxfId="100" headerRowCellStyle="Normal 2">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{38A2B7C7-36B5-0248-9C05-1D30EB7012A6}" name="PR3-E8.2" dataDxfId="99" dataCellStyle="Normal 2"/>
@@ -7309,7 +7006,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4C910E91-0772-5946-8CF6-491D3F781DD4}" name="PolicyR3e83" displayName="PolicyR3e83" ref="A18:K21" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87" tableBorderDxfId="86" headerRowCellStyle="Normal 2">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{B01B4419-95A1-4A4D-A007-B9D68D4BAEEE}" name="PR3- E8.3" dataDxfId="85" dataCellStyle="Normal 2"/>
@@ -7328,7 +7025,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{77C3F932-AF6B-2644-9FE3-9CB36F4B1FC3}" name="PolicyR3e84" displayName="PolicyR3e84" ref="A23:K24" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73" tableBorderDxfId="72" headerRowCellStyle="Normal 2">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{66306BC1-EBE7-DC49-AD9D-014EF58F50F2}" name="PR3-E8.4" dataDxfId="71" dataCellStyle="Normal 2"/>
@@ -7342,6 +7039,22 @@
     <tableColumn id="9" xr3:uid="{1273A66A-0DE4-C846-A632-953F2501882D}" name="Percentage of staff with elevated privileges who do not have a separate standard user account." dataDxfId="63" dataCellStyle="20% - Accent2"/>
     <tableColumn id="10" xr3:uid="{E080A59B-5F00-F347-AF1F-4D9A3F571BC6}" name="Comments" dataDxfId="62" dataCellStyle="Note 2"/>
     <tableColumn id="11" xr3:uid="{8FC89C23-49CA-6C4C-987F-6BC7ADC46147}" name="Column1" dataDxfId="61" dataCellStyle="Note 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6164995D-5379-4B4B-AB4D-A1F7140BC99E}" name="PolicyR3e85" displayName="PolicyR3e85" ref="A26:H27" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" headerRowCellStyle="Normal 2" dataCellStyle="20% - Accent2">
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{CE9FC516-AA87-AA47-BBE7-F770B6728414}" name="PR3-E8.5" dataDxfId="58" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{3669DB3C-1E3A-F141-8792-A74B75841706}" name="Disable untrusted Microsoft Office macros_x000a_Macros are increasingly being used to enable the download of malware.  Adversaries can then access sensitive information, so macros should be secured or disabled" dataDxfId="57" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{C2DABD41-D65D-6641-A127-793B0DC3048B}" name="Additional" dataDxfId="56" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" xr3:uid="{DAAAA271-77B9-AB4B-AAAC-5A162EBFE138}" name="Percentage of fleet with MS Office macros disabled. _x000a_(Compute devices where MSOffice installed are considered 'disabled')" dataDxfId="55" dataCellStyle="20% - Accent2"/>
+    <tableColumn id="5" xr3:uid="{7CEE5809-E85B-2448-AEF5-AC9430FD3194}" name="Risk mitigation for macro enabled workstations (evidence may be required)" dataDxfId="54" dataCellStyle="Note 2"/>
+    <tableColumn id="6" xr3:uid="{E4051793-5F59-9248-B72A-8CE003B38081}" name="Additional Comments (optional)" dataDxfId="53" dataCellStyle="Note 2"/>
+    <tableColumn id="7" xr3:uid="{727CBA5F-574C-9845-BC3A-8F1BDF08B84A}" name="Total percentage of protected fleet   (Cybersecurity Unit to review and accept)" dataDxfId="52" dataCellStyle="20% - Accent2"/>
+    <tableColumn id="8" xr3:uid="{CE3B73D5-AE0F-4B4B-813D-F000612DF1E9}" name="Comments if any" dataDxfId="51" dataCellStyle="20% - Accent2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7652,178 +7365,178 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="46"/>
+    <col min="1" max="16384" width="8.85546875" style="45"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="149" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
     </row>
     <row r="2" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="167"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
-      <c r="H2" s="167"/>
-      <c r="I2" s="167"/>
+      <c r="B2" s="150"/>
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="150"/>
+      <c r="G2" s="150"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="150"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="151" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="159"/>
-      <c r="C3" s="159"/>
-      <c r="D3" s="159"/>
-      <c r="E3" s="159"/>
-      <c r="F3" s="159"/>
-      <c r="G3" s="159"/>
-      <c r="H3" s="159"/>
-      <c r="I3" s="159"/>
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="105"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
+      <c r="A4" s="102"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="169" t="s">
+      <c r="A5" s="153" t="s">
         <v>305</v>
       </c>
-      <c r="B5" s="170"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="170"/>
-      <c r="E5" s="170"/>
-      <c r="F5" s="170"/>
-      <c r="G5" s="170"/>
-      <c r="H5" s="170"/>
-      <c r="I5" s="171"/>
+      <c r="B5" s="154"/>
+      <c r="C5" s="154"/>
+      <c r="D5" s="154"/>
+      <c r="E5" s="154"/>
+      <c r="F5" s="154"/>
+      <c r="G5" s="154"/>
+      <c r="H5" s="154"/>
+      <c r="I5" s="155"/>
     </row>
     <row r="6" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="163" t="s">
+      <c r="A6" s="146" t="s">
         <v>309</v>
       </c>
-      <c r="B6" s="164"/>
-      <c r="C6" s="164"/>
-      <c r="D6" s="164"/>
-      <c r="E6" s="164"/>
-      <c r="F6" s="164"/>
-      <c r="G6" s="164"/>
-      <c r="H6" s="164"/>
-      <c r="I6" s="165"/>
+      <c r="B6" s="147"/>
+      <c r="C6" s="147"/>
+      <c r="D6" s="147"/>
+      <c r="E6" s="147"/>
+      <c r="F6" s="147"/>
+      <c r="G6" s="147"/>
+      <c r="H6" s="147"/>
+      <c r="I6" s="148"/>
     </row>
     <row r="7" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="153" t="s">
+      <c r="A7" s="160" t="s">
         <v>306</v>
       </c>
-      <c r="B7" s="159"/>
-      <c r="C7" s="159"/>
-      <c r="D7" s="159"/>
-      <c r="E7" s="159"/>
-      <c r="F7" s="159"/>
-      <c r="G7" s="159"/>
-      <c r="H7" s="159"/>
-      <c r="I7" s="160"/>
+      <c r="B7" s="152"/>
+      <c r="C7" s="152"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="152"/>
+      <c r="F7" s="152"/>
+      <c r="G7" s="152"/>
+      <c r="H7" s="152"/>
+      <c r="I7" s="166"/>
     </row>
     <row r="8" spans="1:9" ht="63.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="150" t="s">
+      <c r="A8" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="151"/>
-      <c r="C8" s="151"/>
-      <c r="D8" s="151"/>
-      <c r="E8" s="151"/>
-      <c r="F8" s="151"/>
-      <c r="G8" s="151"/>
-      <c r="H8" s="151"/>
-      <c r="I8" s="152"/>
+      <c r="B8" s="158"/>
+      <c r="C8" s="158"/>
+      <c r="D8" s="158"/>
+      <c r="E8" s="158"/>
+      <c r="F8" s="158"/>
+      <c r="G8" s="158"/>
+      <c r="H8" s="158"/>
+      <c r="I8" s="159"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="153" t="s">
+      <c r="A9" s="160" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="154"/>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="154"/>
-      <c r="H9" s="154"/>
-      <c r="I9" s="155"/>
-    </row>
-    <row r="10" spans="1:9" s="47" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="156" t="s">
+      <c r="B9" s="161"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="161"/>
+      <c r="F9" s="161"/>
+      <c r="G9" s="161"/>
+      <c r="H9" s="161"/>
+      <c r="I9" s="162"/>
+    </row>
+    <row r="10" spans="1:9" s="46" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="163" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="157"/>
-      <c r="C10" s="157"/>
-      <c r="D10" s="157"/>
-      <c r="E10" s="157"/>
-      <c r="F10" s="157"/>
-      <c r="G10" s="157"/>
-      <c r="H10" s="157"/>
-      <c r="I10" s="158"/>
-    </row>
-    <row r="11" spans="1:9" s="47" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="161" t="s">
+      <c r="B10" s="164"/>
+      <c r="C10" s="164"/>
+      <c r="D10" s="164"/>
+      <c r="E10" s="164"/>
+      <c r="F10" s="164"/>
+      <c r="G10" s="164"/>
+      <c r="H10" s="164"/>
+      <c r="I10" s="165"/>
+    </row>
+    <row r="11" spans="1:9" s="46" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="167" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="162"/>
-      <c r="C11" s="162"/>
-      <c r="D11" s="162"/>
-      <c r="E11" s="162"/>
-      <c r="F11" s="162"/>
-      <c r="G11" s="162"/>
-      <c r="H11" s="162"/>
-      <c r="I11" s="162"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="168"/>
+      <c r="D11" s="168"/>
+      <c r="E11" s="168"/>
+      <c r="F11" s="168"/>
+      <c r="G11" s="168"/>
+      <c r="H11" s="168"/>
+      <c r="I11" s="168"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="107" t="s">
+      <c r="A12" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="108"/>
-      <c r="C12" s="149" t="s">
+      <c r="B12" s="105"/>
+      <c r="C12" s="156" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="149"/>
-      <c r="E12" s="149"/>
-      <c r="F12" s="149"/>
-      <c r="G12" s="149"/>
-      <c r="H12" s="149"/>
-      <c r="I12" s="149"/>
+      <c r="D12" s="156"/>
+      <c r="E12" s="156"/>
+      <c r="F12" s="156"/>
+      <c r="G12" s="156"/>
+      <c r="H12" s="156"/>
+      <c r="I12" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A5:I5"/>
     <mergeCell ref="C12:I12"/>
     <mergeCell ref="A8:I8"/>
     <mergeCell ref="A9:I9"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A7:I7"/>
     <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A5:I5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{357412D1-D809-42A8-A171-62DB313EA5FE}"/>
@@ -7852,14 +7565,14 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="171" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -7918,14 +7631,14 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="171" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -7989,14 +7702,14 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="171" t="s">
         <v>262</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -8061,14 +7774,14 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="171" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -8136,7 +7849,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="145" t="s">
         <v>331</v>
       </c>
       <c r="B1" s="15"/>
@@ -8167,21 +7880,21 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="171" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="174"/>
-      <c r="C1" s="174"/>
-      <c r="D1" s="174"/>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -8285,134 +7998,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="177" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="183" t="s">
         <v>268</v>
       </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
+      <c r="B2" s="183"/>
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="183"/>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="183" t="s">
         <v>269</v>
       </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
+      <c r="B3" s="183"/>
+      <c r="C3" s="183"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="183"/>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="176" t="s">
+      <c r="A4" s="183" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="176"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="183"/>
+      <c r="D4" s="183"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="I4" s="183"/>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="176" t="s">
+      <c r="A5" s="183" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="176"/>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="176"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="176"/>
-      <c r="H5" s="176"/>
-      <c r="I5" s="176"/>
+      <c r="B5" s="183"/>
+      <c r="C5" s="183"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="177" t="s">
+      <c r="A6" s="185" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="178"/>
-      <c r="C6" s="178"/>
-      <c r="D6" s="179"/>
+      <c r="B6" s="186"/>
+      <c r="C6" s="186"/>
+      <c r="D6" s="187"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="180"/>
-      <c r="G6" s="181"/>
-      <c r="H6" s="181"/>
-      <c r="I6" s="182"/>
+      <c r="F6" s="188"/>
+      <c r="G6" s="189"/>
+      <c r="H6" s="189"/>
+      <c r="I6" s="190"/>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="175" t="s">
+      <c r="A7" s="177" t="s">
         <v>272</v>
       </c>
-      <c r="B7" s="175"/>
-      <c r="C7" s="175"/>
-      <c r="D7" s="175"/>
-      <c r="E7" s="175"/>
-      <c r="F7" s="175"/>
-      <c r="G7" s="175"/>
-      <c r="H7" s="175"/>
-      <c r="I7" s="175"/>
+      <c r="B7" s="177"/>
+      <c r="C7" s="177"/>
+      <c r="D7" s="177"/>
+      <c r="E7" s="177"/>
+      <c r="F7" s="177"/>
+      <c r="G7" s="177"/>
+      <c r="H7" s="177"/>
+      <c r="I7" s="177"/>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="176" t="s">
+      <c r="A8" s="183" t="s">
         <v>273</v>
       </c>
-      <c r="B8" s="176"/>
-      <c r="C8" s="176"/>
-      <c r="D8" s="176"/>
-      <c r="E8" s="176"/>
-      <c r="F8" s="176"/>
-      <c r="G8" s="176"/>
-      <c r="H8" s="176"/>
-      <c r="I8" s="176"/>
+      <c r="B8" s="183"/>
+      <c r="C8" s="183"/>
+      <c r="D8" s="183"/>
+      <c r="E8" s="183"/>
+      <c r="F8" s="183"/>
+      <c r="G8" s="183"/>
+      <c r="H8" s="183"/>
+      <c r="I8" s="183"/>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="175" t="s">
+      <c r="A9" s="177" t="s">
         <v>274</v>
       </c>
-      <c r="B9" s="175"/>
-      <c r="C9" s="175"/>
-      <c r="D9" s="175"/>
-      <c r="E9" s="175"/>
-      <c r="F9" s="175"/>
-      <c r="G9" s="175"/>
-      <c r="H9" s="175"/>
-      <c r="I9" s="175"/>
+      <c r="B9" s="177"/>
+      <c r="C9" s="177"/>
+      <c r="D9" s="177"/>
+      <c r="E9" s="177"/>
+      <c r="F9" s="177"/>
+      <c r="G9" s="177"/>
+      <c r="H9" s="177"/>
+      <c r="I9" s="177"/>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="183" t="s">
+      <c r="A10" s="175" t="s">
         <v>275</v>
       </c>
-      <c r="B10" s="184"/>
-      <c r="C10" s="184"/>
-      <c r="D10" s="184"/>
-      <c r="E10" s="184"/>
-      <c r="F10" s="184"/>
-      <c r="G10" s="184"/>
-      <c r="H10" s="184"/>
-      <c r="I10" s="184"/>
+      <c r="B10" s="176"/>
+      <c r="C10" s="176"/>
+      <c r="D10" s="176"/>
+      <c r="E10" s="176"/>
+      <c r="F10" s="176"/>
+      <c r="G10" s="176"/>
+      <c r="H10" s="176"/>
+      <c r="I10" s="176"/>
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
@@ -8426,43 +8139,43 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="175" t="s">
+      <c r="A12" s="177" t="s">
         <v>276</v>
       </c>
-      <c r="B12" s="175"/>
-      <c r="C12" s="175"/>
-      <c r="D12" s="175"/>
-      <c r="E12" s="175"/>
-      <c r="F12" s="175"/>
-      <c r="G12" s="175"/>
-      <c r="H12" s="175"/>
-      <c r="I12" s="175"/>
+      <c r="B12" s="177"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="177"/>
+      <c r="E12" s="177"/>
+      <c r="F12" s="177"/>
+      <c r="G12" s="177"/>
+      <c r="H12" s="177"/>
+      <c r="I12" s="177"/>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="187" t="s">
+      <c r="A13" s="174" t="s">
         <v>277</v>
       </c>
-      <c r="B13" s="187"/>
-      <c r="C13" s="187"/>
-      <c r="D13" s="187"/>
-      <c r="E13" s="187"/>
-      <c r="F13" s="187"/>
-      <c r="G13" s="187"/>
-      <c r="H13" s="187"/>
-      <c r="I13" s="187"/>
+      <c r="B13" s="174"/>
+      <c r="C13" s="174"/>
+      <c r="D13" s="174"/>
+      <c r="E13" s="174"/>
+      <c r="F13" s="174"/>
+      <c r="G13" s="174"/>
+      <c r="H13" s="174"/>
+      <c r="I13" s="174"/>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="183" t="s">
+      <c r="A14" s="175" t="s">
         <v>278</v>
       </c>
-      <c r="B14" s="184"/>
-      <c r="C14" s="184"/>
-      <c r="D14" s="184"/>
-      <c r="E14" s="184"/>
-      <c r="F14" s="184"/>
-      <c r="G14" s="184"/>
-      <c r="H14" s="184"/>
-      <c r="I14" s="184"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="176"/>
+      <c r="F14" s="176"/>
+      <c r="G14" s="176"/>
+      <c r="H14" s="176"/>
+      <c r="I14" s="176"/>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
@@ -8476,134 +8189,134 @@
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="175" t="s">
+      <c r="A16" s="177" t="s">
         <v>279</v>
       </c>
-      <c r="B16" s="175"/>
-      <c r="C16" s="175"/>
-      <c r="D16" s="175"/>
-      <c r="E16" s="175"/>
-      <c r="F16" s="175"/>
-      <c r="G16" s="175"/>
-      <c r="H16" s="175"/>
-      <c r="I16" s="175"/>
+      <c r="B16" s="177"/>
+      <c r="C16" s="177"/>
+      <c r="D16" s="177"/>
+      <c r="E16" s="177"/>
+      <c r="F16" s="177"/>
+      <c r="G16" s="177"/>
+      <c r="H16" s="177"/>
+      <c r="I16" s="177"/>
     </row>
     <row r="17" spans="1:9" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="188" t="s">
+      <c r="A17" s="178" t="s">
         <v>280</v>
       </c>
-      <c r="B17" s="188"/>
-      <c r="C17" s="188"/>
-      <c r="D17" s="188"/>
-      <c r="E17" s="188"/>
-      <c r="F17" s="188"/>
-      <c r="G17" s="188"/>
-      <c r="H17" s="188"/>
-      <c r="I17" s="188"/>
+      <c r="B17" s="178"/>
+      <c r="C17" s="178"/>
+      <c r="D17" s="178"/>
+      <c r="E17" s="178"/>
+      <c r="F17" s="178"/>
+      <c r="G17" s="178"/>
+      <c r="H17" s="178"/>
+      <c r="I17" s="178"/>
     </row>
     <row r="18" spans="1:9" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="189" t="s">
+      <c r="A18" s="179" t="s">
         <v>281</v>
       </c>
-      <c r="B18" s="190"/>
-      <c r="C18" s="190"/>
-      <c r="D18" s="190"/>
-      <c r="E18" s="190"/>
-      <c r="F18" s="190"/>
-      <c r="G18" s="190"/>
-      <c r="H18" s="190"/>
-      <c r="I18" s="190"/>
+      <c r="B18" s="180"/>
+      <c r="C18" s="180"/>
+      <c r="D18" s="180"/>
+      <c r="E18" s="180"/>
+      <c r="F18" s="180"/>
+      <c r="G18" s="180"/>
+      <c r="H18" s="180"/>
+      <c r="I18" s="180"/>
     </row>
     <row r="19" spans="1:9" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="191" t="s">
+      <c r="A19" s="181" t="s">
         <v>282</v>
       </c>
-      <c r="B19" s="191"/>
-      <c r="C19" s="191"/>
-      <c r="D19" s="191"/>
-      <c r="E19" s="191"/>
-      <c r="F19" s="191"/>
-      <c r="G19" s="191"/>
-      <c r="H19" s="191"/>
-      <c r="I19" s="191"/>
+      <c r="B19" s="181"/>
+      <c r="C19" s="181"/>
+      <c r="D19" s="181"/>
+      <c r="E19" s="181"/>
+      <c r="F19" s="181"/>
+      <c r="G19" s="181"/>
+      <c r="H19" s="181"/>
+      <c r="I19" s="181"/>
     </row>
     <row r="20" spans="1:9" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="192" t="s">
+      <c r="A20" s="182" t="s">
         <v>283</v>
       </c>
-      <c r="B20" s="192"/>
-      <c r="C20" s="192"/>
-      <c r="D20" s="192"/>
-      <c r="E20" s="192"/>
-      <c r="F20" s="192"/>
-      <c r="G20" s="192"/>
-      <c r="H20" s="192"/>
-      <c r="I20" s="192"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="182"/>
     </row>
     <row r="21" spans="1:9" s="2" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="176" t="s">
+      <c r="A21" s="183" t="s">
         <v>284</v>
       </c>
-      <c r="B21" s="176"/>
-      <c r="C21" s="176"/>
-      <c r="D21" s="176"/>
-      <c r="E21" s="176"/>
-      <c r="F21" s="176"/>
-      <c r="G21" s="176"/>
-      <c r="H21" s="176"/>
-      <c r="I21" s="176"/>
+      <c r="B21" s="183"/>
+      <c r="C21" s="183"/>
+      <c r="D21" s="183"/>
+      <c r="E21" s="183"/>
+      <c r="F21" s="183"/>
+      <c r="G21" s="183"/>
+      <c r="H21" s="183"/>
+      <c r="I21" s="183"/>
     </row>
     <row r="22" spans="1:9" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="175" t="s">
+      <c r="A22" s="177" t="s">
         <v>285</v>
       </c>
-      <c r="B22" s="175"/>
-      <c r="C22" s="175"/>
-      <c r="D22" s="175"/>
-      <c r="E22" s="175"/>
-      <c r="F22" s="175"/>
-      <c r="G22" s="175"/>
-      <c r="H22" s="175"/>
-      <c r="I22" s="175"/>
+      <c r="B22" s="177"/>
+      <c r="C22" s="177"/>
+      <c r="D22" s="177"/>
+      <c r="E22" s="177"/>
+      <c r="F22" s="177"/>
+      <c r="G22" s="177"/>
+      <c r="H22" s="177"/>
+      <c r="I22" s="177"/>
     </row>
     <row r="23" spans="1:9" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="193" t="s">
+      <c r="A23" s="184" t="s">
         <v>286</v>
       </c>
-      <c r="B23" s="193"/>
-      <c r="C23" s="193"/>
-      <c r="D23" s="193"/>
-      <c r="E23" s="193"/>
-      <c r="F23" s="193"/>
-      <c r="G23" s="193"/>
-      <c r="H23" s="193"/>
-      <c r="I23" s="193"/>
+      <c r="B23" s="184"/>
+      <c r="C23" s="184"/>
+      <c r="D23" s="184"/>
+      <c r="E23" s="184"/>
+      <c r="F23" s="184"/>
+      <c r="G23" s="184"/>
+      <c r="H23" s="184"/>
+      <c r="I23" s="184"/>
     </row>
     <row r="24" spans="1:9" s="2" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="175" t="s">
+      <c r="A24" s="177" t="s">
         <v>287</v>
       </c>
-      <c r="B24" s="175"/>
-      <c r="C24" s="175"/>
-      <c r="D24" s="175"/>
-      <c r="E24" s="175"/>
-      <c r="F24" s="175"/>
-      <c r="G24" s="175"/>
-      <c r="H24" s="175"/>
-      <c r="I24" s="175"/>
+      <c r="B24" s="177"/>
+      <c r="C24" s="177"/>
+      <c r="D24" s="177"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="177"/>
+      <c r="H24" s="177"/>
+      <c r="I24" s="177"/>
     </row>
     <row r="25" spans="1:9" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="185" t="s">
+      <c r="A25" s="172" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="186"/>
-      <c r="C25" s="186"/>
-      <c r="D25" s="186"/>
-      <c r="E25" s="186"/>
-      <c r="F25" s="186"/>
-      <c r="G25" s="186"/>
-      <c r="H25" s="186"/>
-      <c r="I25" s="186"/>
+      <c r="B25" s="173"/>
+      <c r="C25" s="173"/>
+      <c r="D25" s="173"/>
+      <c r="E25" s="173"/>
+      <c r="F25" s="173"/>
+      <c r="G25" s="173"/>
+      <c r="H25" s="173"/>
+      <c r="I25" s="173"/>
     </row>
     <row r="26" spans="1:9" s="2" customFormat="1" ht="6.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
@@ -8622,6 +8335,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A10:I10"/>
     <mergeCell ref="A25:I25"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="A14:I14"/>
@@ -8634,18 +8359,6 @@
     <mergeCell ref="A22:I22"/>
     <mergeCell ref="A23:I23"/>
     <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A10:I10"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A10" r:id="rId1" display="https://www.qgcio.qld.gov.au/documents/information-security-policy_x000a__x000a_ " xr:uid="{3A93C843-C1FF-41B8-A248-E76E203BCE29}"/>
@@ -8681,14 +8394,14 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="118" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="119" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="25" t="s">
@@ -8697,38 +8410,38 @@
       <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="120" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="120"/>
+      <c r="C4" s="117"/>
     </row>
     <row r="5" spans="1:3" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="121" t="s">
         <v>310</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="C5" s="131" t="s">
+      <c r="C5" s="128" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="119" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>311</v>
       </c>
-      <c r="C6" s="132" t="s">
+      <c r="C6" s="129" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="125" t="s">
+      <c r="A7" s="122" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="20" t="s">
@@ -8736,64 +8449,64 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="126" t="s">
+      <c r="A8" s="123" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="26">
         <v>468463789</v>
       </c>
-      <c r="C8" s="120"/>
+      <c r="C8" s="117"/>
     </row>
     <row r="9" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="127"/>
-      <c r="B9" s="110"/>
+      <c r="A9" s="124"/>
+      <c r="B9" s="107"/>
     </row>
     <row r="10" spans="1:3" ht="78.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="127" t="s">
+      <c r="A10" s="124" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="21">
         <v>0</v>
       </c>
-      <c r="C10" s="129" t="s">
+      <c r="C10" s="126" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="128" t="s">
+      <c r="A11" s="125" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="29">
         <v>0</v>
       </c>
-      <c r="C11" s="133" t="s">
+      <c r="C11" s="130" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="129" t="s">
+      <c r="A12" s="126" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="134"/>
+      <c r="C12" s="131"/>
     </row>
     <row r="13" spans="1:3" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="130"/>
+      <c r="A13" s="127"/>
       <c r="B13" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="135"/>
+      <c r="C13" s="132"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="136" t="s">
+      <c r="A14" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="137" t="s">
+      <c r="B14" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="138"/>
+      <c r="C14" s="135"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8818,156 +8531,153 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="A1:I1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="81" customWidth="1"/>
-    <col min="2" max="6" width="28.85546875" style="81" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" style="81" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" style="81" customWidth="1"/>
-    <col min="9" max="9" width="55.28515625" style="81" customWidth="1"/>
-    <col min="10" max="10" width="0" style="81" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="81"/>
+    <col min="1" max="1" width="37.28515625" style="80" customWidth="1"/>
+    <col min="2" max="6" width="28.85546875" style="80" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" style="80" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" style="80" customWidth="1"/>
+    <col min="9" max="9" width="55.28515625" style="80" customWidth="1"/>
+    <col min="10" max="10" width="0" style="80" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="191" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="102" t="s">
+      <c r="B1" s="191" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="191" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="D1" s="191" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="102" t="s">
+      <c r="E1" s="191" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="102" t="s">
+      <c r="F1" s="191" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="191" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="H1" s="191" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="76" t="s">
+      <c r="I1" s="192" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="76" t="s">
+      <c r="J1" s="193" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="194" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="194" t="s">
         <v>318</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="194" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="194" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="194" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="194" t="s">
         <v>361</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="194" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="194" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="77" t="s">
+      <c r="I2" s="195" t="s">
         <v>295</v>
       </c>
-      <c r="J2" s="103" t="s">
+      <c r="J2" s="196" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="191.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="197" t="s">
         <v>362</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="197" t="s">
         <v>317</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="197" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="197" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="197" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="197" t="s">
         <v>361</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="197" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="197" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="77" t="s">
+      <c r="I3" s="198" t="s">
         <v>297</v>
       </c>
-      <c r="J3" s="103" t="s">
+      <c r="J3" s="199" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="198.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="200" t="s">
         <v>308</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="200" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="200" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="200" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="200" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="200" t="s">
         <v>360</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="200" t="s">
         <v>44</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="200" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="77" t="s">
+      <c r="I4" s="201" t="s">
         <v>296</v>
       </c>
-      <c r="J4" s="103" t="s">
+      <c r="J4" s="196" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -8985,382 +8695,382 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="81"/>
-    <col min="2" max="2" width="21.28515625" style="81" customWidth="1"/>
-    <col min="3" max="3" width="33" style="81" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" style="81" customWidth="1"/>
-    <col min="5" max="6" width="51.85546875" style="81" customWidth="1"/>
-    <col min="7" max="7" width="33.28515625" style="81" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" style="81" customWidth="1"/>
-    <col min="9" max="9" width="17" style="81" hidden="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="81"/>
+    <col min="1" max="1" width="8.85546875" style="80"/>
+    <col min="2" max="2" width="21.28515625" style="80" customWidth="1"/>
+    <col min="3" max="3" width="33" style="80" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" style="80" customWidth="1"/>
+    <col min="5" max="6" width="51.85546875" style="80" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" style="80" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="80" customWidth="1"/>
+    <col min="9" max="9" width="17" style="80" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="80"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="101" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:9" s="100" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="98" t="s">
+      <c r="E1" s="97" t="s">
         <v>322</v>
       </c>
-      <c r="F1" s="98" t="s">
+      <c r="F1" s="97" t="s">
         <v>319</v>
       </c>
-      <c r="G1" s="99" t="s">
+      <c r="G1" s="98" t="s">
         <v>321</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="H1" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="100" t="s">
+      <c r="I1" s="99" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="101" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+    <row r="2" spans="1:9" s="100" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82" t="s">
         <v>302</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="84" t="s">
         <v>298</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="112" t="s">
+      <c r="F2" s="84"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="111"/>
+      <c r="I2" s="108"/>
     </row>
     <row r="3" spans="1:9" ht="266.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="84" t="s">
         <v>328</v>
       </c>
-      <c r="F3" s="85" t="s">
+      <c r="F3" s="84" t="s">
         <v>326</v>
       </c>
-      <c r="G3" s="86"/>
-      <c r="H3" s="140" t="s">
+      <c r="G3" s="85"/>
+      <c r="H3" s="137" t="s">
         <v>339</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="58" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="82" t="s">
+      <c r="B4" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="85" t="s">
+      <c r="E4" s="84" t="s">
         <v>329</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="84" t="s">
+      <c r="F4" s="84"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="59" t="s">
+      <c r="I4" s="58" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="345" x14ac:dyDescent="0.25">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="140" t="s">
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="137" t="s">
         <v>339</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="58" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="195" x14ac:dyDescent="0.25">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="140" t="s">
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="137" t="s">
         <v>339</v>
       </c>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="58" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="89" t="s">
+      <c r="C7" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="142" t="s">
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="139" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="58" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="86" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="88" t="s">
+      <c r="B8" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="82" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="142" t="s">
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="139" t="s">
         <v>341</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="58" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="87" t="s">
+      <c r="A9" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="88" t="s">
+      <c r="B9" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="83" t="s">
+      <c r="C9" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="142" t="s">
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="139" t="s">
         <v>341</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="58" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="A10" s="87" t="s">
+      <c r="A10" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="83" t="s">
+      <c r="C10" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="59" t="s">
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="58" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="63" x14ac:dyDescent="0.25">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="86" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="59" t="s">
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="58" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="86" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="83" t="s">
+      <c r="C12" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="D12" s="82" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="85"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="59" t="s">
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="58" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="87" t="s">
+      <c r="A13" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="88" t="s">
+      <c r="B13" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="83" t="s">
+      <c r="C13" s="82" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="83" t="s">
+      <c r="D13" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="85"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="141" t="s">
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="138" t="s">
         <v>340</v>
       </c>
-      <c r="I13" s="59" t="s">
+      <c r="I13" s="58" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="87" t="s">
+      <c r="A14" s="86" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="88" t="s">
+      <c r="B14" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="83" t="s">
+      <c r="C14" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="D14" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="141" t="s">
+      <c r="E14" s="84"/>
+      <c r="F14" s="84"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="138" t="s">
         <v>340</v>
       </c>
-      <c r="I14" s="59" t="s">
+      <c r="I14" s="58" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="87" t="s">
+      <c r="A15" s="86" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="88" t="s">
+      <c r="B15" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="C15" s="83" t="s">
+      <c r="C15" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="85"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="59" t="s">
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="58" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="91" t="s">
+      <c r="A16" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="93" t="s">
+      <c r="C16" s="92" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="93" t="s">
+      <c r="D16" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="95"/>
-      <c r="F16" s="95"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="94"/>
-      <c r="I16" s="59" t="s">
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="95"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="58" t="s">
         <v>117</v>
       </c>
     </row>
@@ -9401,87 +9111,87 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="75"/>
-    <col min="2" max="2" width="53.7109375" style="75" customWidth="1"/>
-    <col min="3" max="3" width="53.85546875" style="75" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" style="75" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" style="75" customWidth="1"/>
-    <col min="6" max="6" width="28" style="75" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" style="75" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="75"/>
+    <col min="1" max="1" width="8.85546875" style="74"/>
+    <col min="2" max="2" width="53.7109375" style="74" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" style="74" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" style="74" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" style="74" customWidth="1"/>
+    <col min="6" max="6" width="28" style="74" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" style="74" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="77" t="s">
         <v>323</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="77" t="s">
         <v>319</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="77" t="s">
         <v>324</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="G1" s="78" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82" t="s">
         <v>303</v>
       </c>
-      <c r="E2" s="85"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="112" t="s">
+      <c r="E2" s="84"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="109" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="231" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="119" t="s">
+      <c r="D3" s="116" t="s">
         <v>357</v>
       </c>
-      <c r="E3" s="119" t="s">
+      <c r="E3" s="116" t="s">
         <v>356</v>
       </c>
-      <c r="F3" s="77"/>
-      <c r="G3" s="80" t="s">
+      <c r="F3" s="76"/>
+      <c r="G3" s="79" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="87"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="111"/>
-      <c r="I8" s="101"/>
+      <c r="A8" s="86"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="108"/>
+      <c r="I8" s="100"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9489,7 +9199,7 @@
     <hyperlink ref="G2" location="'AuditAssuranceReportTemplate'!A1" display="Audit Assurance Report Template" xr:uid="{83E0E6DE-13A8-4257-A5BF-19FB1696852D}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -9503,879 +9213,879 @@
   </sheetPr>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView topLeftCell="B21" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I38" sqref="B38:I38"/>
+    <sheetView topLeftCell="A18" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="50" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" style="50" customWidth="1"/>
-    <col min="3" max="3" width="32" style="50" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" style="50" customWidth="1"/>
-    <col min="5" max="5" width="64.85546875" style="50" customWidth="1"/>
-    <col min="6" max="6" width="85.7109375" style="50" customWidth="1"/>
-    <col min="7" max="7" width="66.28515625" style="50" customWidth="1"/>
-    <col min="8" max="8" width="85.7109375" style="48" customWidth="1"/>
-    <col min="9" max="9" width="81.140625" style="50" customWidth="1"/>
-    <col min="10" max="10" width="14" style="50" customWidth="1"/>
-    <col min="11" max="11" width="12" style="50" customWidth="1"/>
-    <col min="12" max="16384" width="10.85546875" style="50"/>
+    <col min="1" max="1" width="7.28515625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="32" style="49" customWidth="1"/>
+    <col min="4" max="4" width="53.7109375" style="49" customWidth="1"/>
+    <col min="5" max="5" width="64.85546875" style="49" customWidth="1"/>
+    <col min="6" max="6" width="85.7109375" style="49" customWidth="1"/>
+    <col min="7" max="7" width="66.28515625" style="49" customWidth="1"/>
+    <col min="8" max="8" width="85.7109375" style="47" customWidth="1"/>
+    <col min="9" max="9" width="81.140625" style="49" customWidth="1"/>
+    <col min="10" max="10" width="14" style="49" customWidth="1"/>
+    <col min="11" max="11" width="12" style="49" customWidth="1"/>
+    <col min="12" max="16384" width="10.85546875" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="48" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:11" s="47" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="48" t="s">
         <v>322</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="48" t="s">
         <v>319</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="48" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="48" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="87" t="s">
+    <row r="2" spans="1:11" s="47" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="86" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="C2" s="82" t="s">
         <v>304</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="112"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="109"/>
       <c r="H2" s="12" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="270.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="99" t="s">
         <v>125</v>
       </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="47" t="s">
         <v>359</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
     </row>
     <row r="4" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="47" t="s">
         <v>288</v>
       </c>
-      <c r="D4" s="74"/>
-      <c r="E4" s="48" t="s">
+      <c r="D4" s="73"/>
+      <c r="E4" s="47" t="s">
         <v>342</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="49" t="s">
         <v>325</v>
       </c>
-      <c r="H4" s="48" t="s">
+      <c r="H4" s="47" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="47" t="s">
         <v>289</v>
       </c>
-      <c r="D5" s="74"/>
-      <c r="H5" s="48" t="s">
+      <c r="D5" s="73"/>
+      <c r="H5" s="47" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="47" t="s">
         <v>290</v>
       </c>
-      <c r="D6" s="74"/>
-      <c r="H6" s="48" t="s">
+      <c r="D6" s="73"/>
+      <c r="H6" s="47" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="109"/>
-      <c r="B7" s="109"/>
-      <c r="C7" s="109"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
+      <c r="A7" s="106"/>
+      <c r="B7" s="106"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
     </row>
     <row r="8" spans="1:11" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="72" t="s">
         <v>135</v>
       </c>
-      <c r="B8" s="147" t="s">
+      <c r="B8" s="144" t="s">
         <v>358</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="47" t="s">
         <v>337</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="E8" s="48"/>
-      <c r="H8" s="50"/>
+      <c r="E8" s="47"/>
+      <c r="H8" s="49"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73"/>
-      <c r="B9" s="104"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
       <c r="E9" s="12"/>
-      <c r="H9" s="50"/>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="1:11" ht="107.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="51" t="s">
         <v>140</v>
       </c>
-      <c r="F10" s="52" t="s">
+      <c r="F10" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="55">
         <v>0</v>
       </c>
-      <c r="E11" s="57"/>
-      <c r="F11" s="56">
+      <c r="E11" s="56"/>
+      <c r="F11" s="55">
         <v>0</v>
       </c>
-      <c r="H11" s="50"/>
+      <c r="H11" s="49"/>
     </row>
     <row r="12" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="55">
         <v>0</v>
       </c>
-      <c r="E12" s="57"/>
-      <c r="F12" s="56">
+      <c r="E12" s="56"/>
+      <c r="F12" s="55">
         <v>0</v>
       </c>
-      <c r="H12" s="50"/>
+      <c r="H12" s="49"/>
     </row>
     <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="54"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="56"/>
-      <c r="H13" s="50"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="55"/>
+      <c r="H13" s="49"/>
     </row>
     <row r="14" spans="1:11" ht="95.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="F14" s="52" t="s">
+      <c r="F14" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="G14" s="52" t="s">
+      <c r="G14" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="H14" s="58" t="s">
+      <c r="H14" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="I14" s="52" t="s">
+      <c r="I14" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="J14" s="58" t="s">
+      <c r="J14" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="K14" s="58" t="s">
+      <c r="K14" s="57" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="240" x14ac:dyDescent="0.2">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="D15" s="56">
+      <c r="D15" s="55">
         <v>0</v>
       </c>
-      <c r="E15" s="56">
+      <c r="E15" s="55">
         <v>0</v>
       </c>
-      <c r="F15" s="56">
+      <c r="F15" s="55">
         <v>0</v>
       </c>
-      <c r="G15" s="56">
+      <c r="G15" s="55">
         <v>0</v>
       </c>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
     </row>
     <row r="16" spans="1:11" ht="225" x14ac:dyDescent="0.2">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="54" t="s">
         <v>161</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="54" t="s">
         <v>162</v>
       </c>
-      <c r="D16" s="56">
+      <c r="D16" s="55">
         <v>0</v>
       </c>
-      <c r="E16" s="56">
+      <c r="E16" s="55">
         <v>0</v>
       </c>
-      <c r="F16" s="56">
+      <c r="F16" s="55">
         <v>0</v>
       </c>
-      <c r="G16" s="56">
+      <c r="G16" s="55">
         <v>0</v>
       </c>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="59"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
     </row>
     <row r="17" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="60"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
+      <c r="A17" s="59"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
     </row>
     <row r="18" spans="1:11" ht="168" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="51" t="s">
         <v>164</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="51" t="s">
         <v>165</v>
       </c>
-      <c r="D18" s="52" t="s">
+      <c r="D18" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="52" t="s">
+      <c r="F18" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="G18" s="52" t="s">
+      <c r="G18" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="H18" s="58" t="s">
+      <c r="H18" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="I18" s="52" t="s">
+      <c r="I18" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="J18" s="58" t="s">
+      <c r="J18" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="K18" s="58" t="s">
+      <c r="K18" s="57" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="165" x14ac:dyDescent="0.2">
-      <c r="A19" s="62" t="s">
+      <c r="A19" s="61" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="C19" s="55" t="s">
+      <c r="C19" s="54" t="s">
         <v>170</v>
       </c>
-      <c r="D19" s="56">
+      <c r="D19" s="55">
         <v>0</v>
       </c>
-      <c r="E19" s="56">
+      <c r="E19" s="55">
         <v>0</v>
       </c>
-      <c r="F19" s="56">
+      <c r="F19" s="55">
         <v>0</v>
       </c>
-      <c r="G19" s="56">
+      <c r="G19" s="55">
         <v>0</v>
       </c>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
     </row>
     <row r="20" spans="1:11" ht="180" x14ac:dyDescent="0.2">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="61" t="s">
         <v>171</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="54" t="s">
         <v>172</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="D20" s="56">
+      <c r="D20" s="55">
         <v>0</v>
       </c>
-      <c r="E20" s="56">
+      <c r="E20" s="55">
         <v>0</v>
       </c>
-      <c r="F20" s="56">
+      <c r="F20" s="55">
         <v>0</v>
       </c>
-      <c r="G20" s="56">
+      <c r="G20" s="55">
         <v>0</v>
       </c>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="59"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
     </row>
     <row r="21" spans="1:11" ht="165" x14ac:dyDescent="0.2">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="62" t="s">
         <v>174</v>
       </c>
-      <c r="B21" s="55" t="s">
+      <c r="B21" s="54" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="54" t="s">
         <v>170</v>
       </c>
-      <c r="D21" s="56">
+      <c r="D21" s="55">
         <v>0</v>
       </c>
-      <c r="E21" s="56">
+      <c r="E21" s="55">
         <v>0</v>
       </c>
-      <c r="F21" s="56">
+      <c r="F21" s="55">
         <v>0</v>
       </c>
-      <c r="G21" s="56">
+      <c r="G21" s="55">
         <v>0</v>
       </c>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="58"/>
     </row>
     <row r="22" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="64"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="59"/>
-      <c r="K22" s="59"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
     </row>
     <row r="23" spans="1:11" ht="140.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="60" t="s">
         <v>176</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="51" t="s">
         <v>177</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="D23" s="52" t="s">
+      <c r="D23" s="51" t="s">
         <v>179</v>
       </c>
-      <c r="E23" s="52" t="s">
+      <c r="E23" s="51" t="s">
         <v>180</v>
       </c>
-      <c r="F23" s="58" t="s">
+      <c r="F23" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="G23" s="52" t="s">
+      <c r="G23" s="51" t="s">
         <v>182</v>
       </c>
-      <c r="H23" s="52" t="s">
+      <c r="H23" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="I23" s="52" t="s">
+      <c r="I23" s="51" t="s">
         <v>184</v>
       </c>
-      <c r="J23" s="58" t="s">
+      <c r="J23" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="K23" s="58" t="s">
+      <c r="K23" s="57" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="78.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="63" t="s">
+      <c r="A24" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="54" t="s">
         <v>187</v>
       </c>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="56">
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="55">
         <v>0</v>
       </c>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
     </row>
     <row r="25" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="60"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
     </row>
     <row r="26" spans="1:11" ht="138" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="51" t="s">
+      <c r="A26" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="B26" s="52" t="s">
+      <c r="B26" s="51" t="s">
         <v>189</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="D26" s="52" t="s">
+      <c r="D26" s="51" t="s">
         <v>332</v>
       </c>
-      <c r="E26" s="52" t="s">
+      <c r="E26" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="F26" s="52" t="s">
+      <c r="F26" s="51" t="s">
         <v>333</v>
       </c>
-      <c r="G26" s="52" t="s">
+      <c r="G26" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="H26" s="52" t="s">
+      <c r="H26" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="I26" s="53"/>
-      <c r="J26" s="173" t="s">
+      <c r="I26" s="52"/>
+      <c r="J26" s="170" t="s">
         <v>155</v>
       </c>
-      <c r="K26" s="173"/>
+      <c r="K26" s="170"/>
     </row>
     <row r="27" spans="1:11" ht="90.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="54" t="s">
         <v>193</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="54" t="s">
         <v>194</v>
       </c>
-      <c r="D27" s="56">
+      <c r="D27" s="55">
         <v>0</v>
       </c>
-      <c r="E27" s="67" t="s">
+      <c r="E27" s="66" t="s">
         <v>195</v>
       </c>
-      <c r="F27" s="57"/>
-      <c r="G27" s="56">
+      <c r="F27" s="56"/>
+      <c r="G27" s="55">
         <v>0</v>
       </c>
-      <c r="H27" s="56"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="172"/>
-      <c r="K27" s="172"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="169"/>
+      <c r="K27" s="169"/>
     </row>
     <row r="28" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="60"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59"/>
+      <c r="A28" s="59"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="55"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
     </row>
     <row r="29" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="C29" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="D29" s="52" t="s">
+      <c r="D29" s="51" t="s">
         <v>198</v>
       </c>
-      <c r="E29" s="52" t="s">
+      <c r="E29" s="51" t="s">
         <v>199</v>
       </c>
-      <c r="F29" s="52" t="s">
+      <c r="F29" s="51" t="s">
         <v>200</v>
       </c>
-      <c r="G29" s="52" t="s">
+      <c r="G29" s="51" t="s">
         <v>201</v>
       </c>
-      <c r="H29" s="58" t="s">
+      <c r="H29" s="57" t="s">
         <v>202</v>
       </c>
-      <c r="I29" s="58" t="s">
+      <c r="I29" s="57" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.2">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="53" t="s">
         <v>203</v>
       </c>
-      <c r="B30" s="55" t="s">
+      <c r="B30" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="C30" s="55" t="s">
+      <c r="C30" s="54" t="s">
         <v>205</v>
       </c>
-      <c r="D30" s="56">
+      <c r="D30" s="55">
         <v>0</v>
       </c>
-      <c r="E30" s="56">
+      <c r="E30" s="55">
         <v>0</v>
       </c>
-      <c r="F30" s="56">
+      <c r="F30" s="55">
         <v>0</v>
       </c>
-      <c r="G30" s="66"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="59"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="58"/>
     </row>
     <row r="31" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="60"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="59"/>
+      <c r="A31" s="59"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
     </row>
     <row r="32" spans="1:11" ht="98.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="51" t="s">
+      <c r="A32" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="B32" s="52" t="s">
+      <c r="B32" s="51" t="s">
         <v>207</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="52" t="s">
+      <c r="D32" s="51" t="s">
         <v>208</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="F32" s="139" t="s">
+      <c r="F32" s="136" t="s">
         <v>336</v>
       </c>
-      <c r="G32" s="52" t="s">
+      <c r="G32" s="51" t="s">
         <v>210</v>
       </c>
-      <c r="H32" s="52" t="s">
+      <c r="H32" s="51" t="s">
         <v>334</v>
       </c>
-      <c r="I32" s="52"/>
+      <c r="I32" s="51"/>
     </row>
     <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="53" t="s">
         <v>211</v>
       </c>
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="C33" s="55" t="s">
+      <c r="C33" s="54" t="s">
         <v>213</v>
       </c>
-      <c r="D33" s="56">
+      <c r="D33" s="55">
         <v>0</v>
       </c>
-      <c r="E33" s="57"/>
-      <c r="F33" s="69">
+      <c r="E33" s="56"/>
+      <c r="F33" s="68">
         <v>0</v>
       </c>
-      <c r="G33" s="56">
+      <c r="G33" s="55">
         <v>0</v>
       </c>
-      <c r="H33" s="70"/>
-      <c r="I33" s="70"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
     </row>
     <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="53" t="s">
         <v>214</v>
       </c>
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="C34" s="55" t="s">
+      <c r="C34" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="D34" s="56">
+      <c r="D34" s="55">
         <v>0</v>
       </c>
-      <c r="E34" s="57"/>
-      <c r="F34" s="69">
+      <c r="E34" s="56"/>
+      <c r="F34" s="68">
         <v>0</v>
       </c>
-      <c r="G34" s="56">
+      <c r="G34" s="55">
         <v>0</v>
       </c>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
     </row>
     <row r="35" spans="1:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="A35" s="54" t="s">
+      <c r="A35" s="53" t="s">
         <v>217</v>
       </c>
-      <c r="B35" s="55" t="s">
+      <c r="B35" s="54" t="s">
         <v>218</v>
       </c>
-      <c r="C35" s="55" t="s">
+      <c r="C35" s="54" t="s">
         <v>219</v>
       </c>
-      <c r="D35" s="56">
+      <c r="D35" s="55">
         <v>0</v>
       </c>
-      <c r="E35" s="57"/>
-      <c r="F35" s="69">
+      <c r="E35" s="56"/>
+      <c r="F35" s="68">
         <v>0</v>
       </c>
-      <c r="G35" s="56">
+      <c r="G35" s="55">
         <v>0</v>
       </c>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
     </row>
     <row r="36" spans="1:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="A36" s="54" t="s">
+      <c r="A36" s="53" t="s">
         <v>220</v>
       </c>
-      <c r="B36" s="55" t="s">
+      <c r="B36" s="54" t="s">
         <v>221</v>
       </c>
-      <c r="C36" s="55" t="s">
+      <c r="C36" s="54" t="s">
         <v>222</v>
       </c>
-      <c r="D36" s="56">
+      <c r="D36" s="55">
         <v>0</v>
       </c>
-      <c r="E36" s="57"/>
-      <c r="F36" s="69">
+      <c r="E36" s="56"/>
+      <c r="F36" s="68">
         <v>0</v>
       </c>
-      <c r="G36" s="56">
+      <c r="G36" s="55">
         <v>0</v>
       </c>
-      <c r="H36" s="70"/>
-      <c r="I36" s="70"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="69"/>
     </row>
     <row r="37" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="60"/>
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="59"/>
+      <c r="A37" s="59"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="55"/>
+      <c r="I37" s="55"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
     </row>
     <row r="38" spans="1:11" ht="109.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="50" t="s">
         <v>223</v>
       </c>
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="51" t="s">
         <v>224</v>
       </c>
-      <c r="C38" s="52" t="s">
+      <c r="C38" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="57" t="s">
         <v>225</v>
       </c>
-      <c r="E38" s="52" t="s">
+      <c r="E38" s="51" t="s">
         <v>226</v>
       </c>
-      <c r="F38" s="52" t="s">
+      <c r="F38" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="G38" s="52" t="s">
+      <c r="G38" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="H38" s="52" t="s">
+      <c r="H38" s="51" t="s">
         <v>335</v>
       </c>
-      <c r="I38" s="58" t="s">
+      <c r="I38" s="57" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.2">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="53" t="s">
         <v>229</v>
       </c>
-      <c r="B39" s="55" t="s">
+      <c r="B39" s="54" t="s">
         <v>230</v>
       </c>
-      <c r="C39" s="55" t="s">
+      <c r="C39" s="54" t="s">
         <v>231</v>
       </c>
-      <c r="D39" s="56">
+      <c r="D39" s="55">
         <v>0</v>
       </c>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="56">
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="55">
         <v>0</v>
       </c>
-      <c r="I39" s="56">
+      <c r="I39" s="55">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.2">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="53" t="s">
         <v>232</v>
       </c>
-      <c r="B40" s="55" t="s">
+      <c r="B40" s="54" t="s">
         <v>233</v>
       </c>
-      <c r="C40" s="55" t="s">
+      <c r="C40" s="54" t="s">
         <v>234</v>
       </c>
-      <c r="D40" s="56">
+      <c r="D40" s="55">
         <v>0</v>
       </c>
-      <c r="E40" s="57"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="56">
+      <c r="E40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="55">
         <v>0</v>
       </c>
-      <c r="I40" s="56">
+      <c r="I40" s="55">
         <v>0</v>
       </c>
     </row>
@@ -10442,52 +10152,52 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="42"/>
-    <col min="2" max="3" width="51.28515625" style="42" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" style="42" customWidth="1"/>
-    <col min="5" max="5" width="45" style="42" customWidth="1"/>
-    <col min="6" max="6" width="29.140625" style="42" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" style="42" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="42"/>
+    <col min="1" max="1" width="8.85546875" style="41"/>
+    <col min="2" max="3" width="51.28515625" style="41" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" style="41" customWidth="1"/>
+    <col min="5" max="5" width="45" style="41" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" style="41" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="41" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>319</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="39" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="86" t="s">
         <v>330</v>
       </c>
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82" t="s">
         <v>300</v>
       </c>
-      <c r="E2" s="85"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="113" t="s">
+      <c r="E2" s="84"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="110" t="s">
         <v>55</v>
       </c>
     </row>
@@ -10504,20 +10214,20 @@
       <c r="D3" s="32" t="s">
         <v>299</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="F3" s="44"/>
-      <c r="G3" s="114"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="111"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="115"/>
-      <c r="B4" s="116"/>
+      <c r="A4" s="112"/>
+      <c r="B4" s="113"/>
       <c r="C4" s="32"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="114"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="111"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -10554,19 +10264,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="33" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>240</v>
       </c>
     </row>
@@ -10577,13 +10287,13 @@
       <c r="B2" s="31" t="s">
         <v>242</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="35" t="s">
         <v>301</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>327</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="44" t="s">
         <v>243</v>
       </c>
     </row>
@@ -10617,10 +10327,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="142" t="s">
         <v>352</v>
       </c>
-      <c r="C1" s="146" t="s">
+      <c r="C1" s="143" t="s">
         <v>244</v>
       </c>
     </row>
@@ -10648,7 +10358,7 @@
       <c r="B6" s="18" t="s">
         <v>354</v>
       </c>
-      <c r="C6" s="144" t="s">
+      <c r="C6" s="141" t="s">
         <v>7</v>
       </c>
     </row>
@@ -10717,7 +10427,7 @@
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="2:10" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="143" t="s">
+      <c r="B15" s="140" t="s">
         <v>355</v>
       </c>
       <c r="J15" s="12"/>
@@ -10785,6 +10495,43 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="474a08bd-ae9f-4ab7-ab72-cad3c4647737">
+      <UserInfo>
+        <DisplayName>Andy Stokes</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Daniel Klaser</DisplayName>
+        <AccountId>98</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Dinar Adnan</DisplayName>
+        <AccountId>35</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2ea85696-5d49-4719-8940-b51507ccf115">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="474a08bd-ae9f-4ab7-ab72-cad3c4647737" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002E1479B33370014A94629D14E7E035B7" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3f8dbca6bf93f2782719d40778ede3cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="474a08bd-ae9f-4ab7-ab72-cad3c4647737" xmlns:ns3="2ea85696-5d49-4719-8940-b51507ccf115" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c46fde71e1d41f3ccbfaee5083d86d4b" ns2:_="" ns3:_="">
     <xsd:import namespace="474a08bd-ae9f-4ab7-ab72-cad3c4647737"/>
@@ -11027,44 +10774,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29FDB849-2D35-4D47-8357-5A24A389B99C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="474a08bd-ae9f-4ab7-ab72-cad3c4647737"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2ea85696-5d49-4719-8940-b51507ccf115"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="474a08bd-ae9f-4ab7-ab72-cad3c4647737">
-      <UserInfo>
-        <DisplayName>Andy Stokes</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Daniel Klaser</DisplayName>
-        <AccountId>98</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Dinar Adnan</DisplayName>
-        <AccountId>35</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2ea85696-5d49-4719-8940-b51507ccf115">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="474a08bd-ae9f-4ab7-ab72-cad3c4647737" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D19D8D15-F34E-4DDB-A4D5-9901CB38744B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A0ADE18-14C1-4E39-A33A-3D26FDF4A566}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11081,29 +10816,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D19D8D15-F34E-4DDB-A4D5-9901CB38744B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29FDB849-2D35-4D47-8357-5A24A389B99C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="474a08bd-ae9f-4ab7-ab72-cad3c4647737"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2ea85696-5d49-4719-8940-b51507ccf115"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>